<commit_message>
Se agrego la documentación
</commit_message>
<xml_diff>
--- a/Lab/practica1/datos/datos.xlsx
+++ b/Lab/practica1/datos/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joddie\Documents\RepositoriosGitlab\IA\Lab\practica1\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31FAD6D-4555-4AB1-96C4-D98F7555AAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BC9A62-CE58-42A5-BF07-6589305EB4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>CUI</t>
   </si>
@@ -43,16 +43,30 @@
   </si>
   <si>
     <t>Descripción de UIPath201602790</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>jers.033@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,15 +89,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -362,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -374,9 +391,10 @@
     <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,8 +407,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>2098807910101</v>
       </c>
@@ -403,9 +424,15 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D7B0A799-63F4-44C6-8D14-B175A437CFC4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aumento de delay para el directo en fb
</commit_message>
<xml_diff>
--- a/Lab/practica1/datos/datos.xlsx
+++ b/Lab/practica1/datos/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joddie\Documents\RepositoriosGitlab\IA\Lab\practica1\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BC9A62-CE58-42A5-BF07-6589305EB4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA45011-D145-415F-B9B7-C912EE81E388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>CUI</t>
   </si>
@@ -42,13 +42,16 @@
     <t>UIPath201115018</t>
   </si>
   <si>
-    <t>Descripción de UIPath201602790</t>
-  </si>
-  <si>
     <t>Correo</t>
   </si>
   <si>
     <t>jers.033@gmail.com</t>
+  </si>
+  <si>
+    <t>anaisabelculajay@gmail.com</t>
+  </si>
+  <si>
+    <t>Descripción de UIPath201115018</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -394,7 +397,7 @@
     <col min="5" max="5" width="17.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,10 +411,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>2098807910101</v>
       </c>
@@ -422,15 +425,18 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{D7B0A799-63F4-44C6-8D14-B175A437CFC4}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{5FAFA054-5A4C-4F95-91FB-B02D5709BDF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Se agregaron algoritmos a clase y practica 2 al lab
</commit_message>
<xml_diff>
--- a/Lab/practica1/datos/datos.xlsx
+++ b/Lab/practica1/datos/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joddie\Documents\RepositoriosGitlab\IA\Lab\practica1\datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA45011-D145-415F-B9B7-C912EE81E388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDB1BE7-8238-46F8-9447-42741EF3F80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>CUI</t>
   </si>
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -397,7 +397,7 @@
     <col min="5" max="5" width="17.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>2098807910101</v>
       </c>
@@ -427,18 +427,22 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{5FAFA054-5A4C-4F95-91FB-B02D5709BDF2}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{A207B26B-E535-4B24-9B32-CD56685906B1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>